<commit_message>
chore: using sqlite3 instead of excel file as data base
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -452,12 +452,20 @@
       <c r="B30" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30" s="3" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1" s="2">
       <c r="B31" s="3" t="n"/>
+    </row>
+    <row r="32">
+      <c r="B32" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="33" ht="12.75" customHeight="1" s="2">
       <c r="B33" s="3" t="n"/>

</xml_diff>